<commit_message>
Renamed package: archimeded -> archimedes
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java Projects\excel4j\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD02356-7CEB-4DAC-8A45-381CCD6B677F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4827AD36-8A8E-4BD3-B50E-7AAA3EE35095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DBF98241-6752-4E53-86CB-DFFA1B9A0C84}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Name</t>
   </si>
@@ -71,13 +71,10 @@
     <t>List</t>
   </si>
   <si>
-    <t>1;2;3;4</t>
-  </si>
-  <si>
-    <t>1;2;3;5</t>
-  </si>
-  <si>
-    <t>1;2;3;6</t>
+    <t>ayush;deepanshu;aryan;sumit</t>
+  </si>
+  <si>
+    <t>Quantity</t>
   </si>
 </sst>
 </file>
@@ -456,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEAE4181-6C23-4292-8D3C-9D40757681D1}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -469,7 +466,7 @@
     <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -485,8 +482,11 @@
       <c r="E1" t="s">
         <v>10</v>
       </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -502,8 +502,11 @@
       <c r="E2" t="s">
         <v>11</v>
       </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -517,10 +520,13 @@
         <v>42282</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -534,7 +540,10 @@
         <v>42282</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="F4">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>